<commit_message>
#97 Fixed timeOverlapping conflict calculation
It was a renamed object deconstruction that I forgot to change
</commit_message>
<xml_diff>
--- a/Files/data/Calculando conflito de salas.xlsx
+++ b/Files/data/Calculando conflito de salas.xlsx
@@ -8,33 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\timetabling-UENF\Files\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B60F5481-265B-4CD7-BFD5-C7090B259CD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{450E2A4F-79EF-4402-BEEE-5B729D8B3124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8CCE4AE8-80CB-4800-8AEA-6F64646DD493}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="novo caso" sheetId="2" r:id="rId1"/>
+    <sheet name="Planilha1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="30">
   <si>
     <t>Turma A</t>
   </si>
@@ -130,7 +122,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,8 +136,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -188,6 +187,42 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -201,18 +236,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,11 +569,1099 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58C6EC03-9025-4593-B289-11A0D37ABF38}">
+  <dimension ref="A1:H38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="47.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <f>A3+B3</f>
+        <v>8</v>
+      </c>
+      <c r="D3" s="9">
+        <v>7</v>
+      </c>
+      <c r="E3" s="9">
+        <v>1</v>
+      </c>
+      <c r="F3" s="9">
+        <v>8</v>
+      </c>
+      <c r="G3" s="15" t="str">
+        <f>IF(OR(C3&lt;=D3,F3&lt;=A3,B3=0,E3=0),"OK","Conflito")</f>
+        <v>Conflito</v>
+      </c>
+      <c r="H3" s="16" t="str">
+        <f>IF(OR(C3&lt;=D3,F3&lt;=A3,B3=0,E3=0),"true","false")</f>
+        <v>false</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2">
+        <f t="shared" ref="C4:C8" si="0">A4+B4</f>
+        <v>8</v>
+      </c>
+      <c r="D4" s="9">
+        <v>10</v>
+      </c>
+      <c r="E4" s="9">
+        <v>3</v>
+      </c>
+      <c r="F4" s="9">
+        <f>D4+E4</f>
+        <v>13</v>
+      </c>
+      <c r="G4" t="str">
+        <f>IF(OR(C4&lt;=D4,F4&lt;=A4,B4=0,E4=0),"OK","Conflito")</f>
+        <v>OK</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" ref="H4:H38" si="1">IF(OR(C4&lt;=D4,F4&lt;=A4,B4=0,E4=0),"true","false")</f>
+        <v>true</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D5" s="9">
+        <v>12</v>
+      </c>
+      <c r="E5" s="9">
+        <v>5</v>
+      </c>
+      <c r="F5" s="9">
+        <f t="shared" ref="F5:F8" si="2">D5+E5</f>
+        <v>17</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" ref="G4:G38" si="3">IF(OR(C5&lt;=D5,F5&lt;=A5,B5=0,E5=0),"OK","Conflito")</f>
+        <v>OK</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="1"/>
+        <v>true</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D6" s="9">
+        <v>16</v>
+      </c>
+      <c r="E6" s="9">
+        <v>2</v>
+      </c>
+      <c r="F6" s="9">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="1"/>
+        <v>true</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D7" s="9">
+        <v>20</v>
+      </c>
+      <c r="E7" s="9">
+        <v>3</v>
+      </c>
+      <c r="F7" s="9">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="1"/>
+        <v>true</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D8" s="9">
+        <v>21</v>
+      </c>
+      <c r="E8" s="9">
+        <v>0</v>
+      </c>
+      <c r="F8" s="9">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="1"/>
+        <v>true</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="5">
+        <v>10</v>
+      </c>
+      <c r="B9" s="5">
+        <v>3</v>
+      </c>
+      <c r="C9" s="5">
+        <v>13</v>
+      </c>
+      <c r="D9" s="5">
+        <v>7</v>
+      </c>
+      <c r="E9" s="5">
+        <v>1</v>
+      </c>
+      <c r="F9" s="5">
+        <v>8</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="1"/>
+        <v>true</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="5">
+        <v>10</v>
+      </c>
+      <c r="B10" s="5">
+        <v>3</v>
+      </c>
+      <c r="C10" s="5">
+        <v>13</v>
+      </c>
+      <c r="D10" s="5">
+        <v>10</v>
+      </c>
+      <c r="E10" s="5">
+        <v>3</v>
+      </c>
+      <c r="F10" s="5">
+        <v>13</v>
+      </c>
+      <c r="G10" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Conflito</v>
+      </c>
+      <c r="H10" s="16" t="str">
+        <f t="shared" si="1"/>
+        <v>false</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5">
+        <v>3</v>
+      </c>
+      <c r="C11" s="5">
+        <v>13</v>
+      </c>
+      <c r="D11" s="5">
+        <v>12</v>
+      </c>
+      <c r="E11" s="5">
+        <v>5</v>
+      </c>
+      <c r="F11" s="5">
+        <v>17</v>
+      </c>
+      <c r="G11" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>Conflito</v>
+      </c>
+      <c r="H11" s="16" t="str">
+        <f t="shared" si="1"/>
+        <v>false</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="5">
+        <v>10</v>
+      </c>
+      <c r="B12" s="5">
+        <v>3</v>
+      </c>
+      <c r="C12" s="5">
+        <v>13</v>
+      </c>
+      <c r="D12" s="5">
+        <v>16</v>
+      </c>
+      <c r="E12" s="5">
+        <v>2</v>
+      </c>
+      <c r="F12" s="5">
+        <v>18</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="1"/>
+        <v>true</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="5">
+        <v>10</v>
+      </c>
+      <c r="B13" s="5">
+        <v>3</v>
+      </c>
+      <c r="C13" s="5">
+        <v>13</v>
+      </c>
+      <c r="D13" s="5">
+        <v>20</v>
+      </c>
+      <c r="E13" s="5">
+        <v>3</v>
+      </c>
+      <c r="F13" s="5">
+        <v>23</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="1"/>
+        <v>true</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="5">
+        <v>10</v>
+      </c>
+      <c r="B14" s="5">
+        <v>3</v>
+      </c>
+      <c r="C14" s="5">
+        <v>13</v>
+      </c>
+      <c r="D14" s="5">
+        <v>21</v>
+      </c>
+      <c r="E14" s="5">
+        <v>0</v>
+      </c>
+      <c r="F14" s="5">
+        <v>21</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="1"/>
+        <v>true</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="10">
+        <v>12</v>
+      </c>
+      <c r="B15" s="10">
+        <v>5</v>
+      </c>
+      <c r="C15" s="10">
+        <v>17</v>
+      </c>
+      <c r="D15" s="10">
+        <v>7</v>
+      </c>
+      <c r="E15" s="10">
+        <v>1</v>
+      </c>
+      <c r="F15" s="10">
+        <v>8</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="1"/>
+        <v>true</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="10">
+        <v>12</v>
+      </c>
+      <c r="B16" s="10">
+        <v>5</v>
+      </c>
+      <c r="C16" s="10">
+        <v>17</v>
+      </c>
+      <c r="D16" s="10">
+        <v>10</v>
+      </c>
+      <c r="E16" s="10">
+        <v>3</v>
+      </c>
+      <c r="F16" s="10">
+        <v>13</v>
+      </c>
+      <c r="G16" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>Conflito</v>
+      </c>
+      <c r="H16" s="16" t="str">
+        <f t="shared" si="1"/>
+        <v>false</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="10">
+        <v>12</v>
+      </c>
+      <c r="B17" s="10">
+        <v>5</v>
+      </c>
+      <c r="C17" s="10">
+        <v>17</v>
+      </c>
+      <c r="D17" s="10">
+        <v>12</v>
+      </c>
+      <c r="E17" s="10">
+        <v>5</v>
+      </c>
+      <c r="F17" s="10">
+        <v>17</v>
+      </c>
+      <c r="G17" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Conflito</v>
+      </c>
+      <c r="H17" s="16" t="str">
+        <f t="shared" si="1"/>
+        <v>false</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="10">
+        <v>12</v>
+      </c>
+      <c r="B18" s="10">
+        <v>5</v>
+      </c>
+      <c r="C18" s="10">
+        <v>17</v>
+      </c>
+      <c r="D18" s="10">
+        <v>16</v>
+      </c>
+      <c r="E18" s="10">
+        <v>2</v>
+      </c>
+      <c r="F18" s="10">
+        <v>18</v>
+      </c>
+      <c r="G18" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>Conflito</v>
+      </c>
+      <c r="H18" s="16" t="str">
+        <f t="shared" si="1"/>
+        <v>false</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="10">
+        <v>12</v>
+      </c>
+      <c r="B19" s="10">
+        <v>5</v>
+      </c>
+      <c r="C19" s="10">
+        <v>17</v>
+      </c>
+      <c r="D19" s="11">
+        <v>20</v>
+      </c>
+      <c r="E19" s="11">
+        <v>3</v>
+      </c>
+      <c r="F19" s="11">
+        <v>23</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="1"/>
+        <v>true</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="10">
+        <v>12</v>
+      </c>
+      <c r="B20" s="10">
+        <v>5</v>
+      </c>
+      <c r="C20" s="10">
+        <v>17</v>
+      </c>
+      <c r="D20" s="11">
+        <v>21</v>
+      </c>
+      <c r="E20" s="11">
+        <v>0</v>
+      </c>
+      <c r="F20" s="11">
+        <v>21</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="1"/>
+        <v>true</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="12">
+        <v>16</v>
+      </c>
+      <c r="B21" s="12">
+        <v>2</v>
+      </c>
+      <c r="C21" s="12">
+        <v>18</v>
+      </c>
+      <c r="D21" s="12">
+        <v>7</v>
+      </c>
+      <c r="E21" s="12">
+        <v>1</v>
+      </c>
+      <c r="F21" s="12">
+        <v>8</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="1"/>
+        <v>true</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="12">
+        <v>16</v>
+      </c>
+      <c r="B22" s="12">
+        <v>2</v>
+      </c>
+      <c r="C22" s="12">
+        <v>18</v>
+      </c>
+      <c r="D22" s="12">
+        <v>10</v>
+      </c>
+      <c r="E22" s="12">
+        <v>3</v>
+      </c>
+      <c r="F22" s="12">
+        <v>13</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+      <c r="H22" t="str">
+        <f t="shared" si="1"/>
+        <v>true</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="12">
+        <v>16</v>
+      </c>
+      <c r="B23" s="12">
+        <v>2</v>
+      </c>
+      <c r="C23" s="12">
+        <v>18</v>
+      </c>
+      <c r="D23" s="12">
+        <v>12</v>
+      </c>
+      <c r="E23" s="12">
+        <v>5</v>
+      </c>
+      <c r="F23" s="12">
+        <v>17</v>
+      </c>
+      <c r="G23" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>Conflito</v>
+      </c>
+      <c r="H23" s="16" t="str">
+        <f t="shared" si="1"/>
+        <v>false</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="12">
+        <v>16</v>
+      </c>
+      <c r="B24" s="12">
+        <v>2</v>
+      </c>
+      <c r="C24" s="12">
+        <v>18</v>
+      </c>
+      <c r="D24" s="12">
+        <v>16</v>
+      </c>
+      <c r="E24" s="12">
+        <v>2</v>
+      </c>
+      <c r="F24" s="12">
+        <v>18</v>
+      </c>
+      <c r="G24" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Conflito</v>
+      </c>
+      <c r="H24" s="16" t="str">
+        <f t="shared" si="1"/>
+        <v>false</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="12">
+        <v>16</v>
+      </c>
+      <c r="B25" s="12">
+        <v>2</v>
+      </c>
+      <c r="C25" s="12">
+        <v>18</v>
+      </c>
+      <c r="D25" s="12">
+        <v>20</v>
+      </c>
+      <c r="E25" s="12">
+        <v>3</v>
+      </c>
+      <c r="F25" s="12">
+        <v>23</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+      <c r="H25" t="str">
+        <f t="shared" si="1"/>
+        <v>true</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="12">
+        <v>16</v>
+      </c>
+      <c r="B26" s="12">
+        <v>2</v>
+      </c>
+      <c r="C26" s="12">
+        <v>18</v>
+      </c>
+      <c r="D26" s="12">
+        <v>21</v>
+      </c>
+      <c r="E26" s="12">
+        <v>0</v>
+      </c>
+      <c r="F26" s="12">
+        <v>21</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+      <c r="H26" t="str">
+        <f t="shared" si="1"/>
+        <v>true</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="13">
+        <v>20</v>
+      </c>
+      <c r="B27" s="13">
+        <v>3</v>
+      </c>
+      <c r="C27" s="13">
+        <v>23</v>
+      </c>
+      <c r="D27" s="13">
+        <v>7</v>
+      </c>
+      <c r="E27" s="13">
+        <v>1</v>
+      </c>
+      <c r="F27" s="13">
+        <v>8</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+      <c r="H27" t="str">
+        <f t="shared" si="1"/>
+        <v>true</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="13">
+        <v>20</v>
+      </c>
+      <c r="B28" s="13">
+        <v>3</v>
+      </c>
+      <c r="C28" s="13">
+        <v>23</v>
+      </c>
+      <c r="D28" s="13">
+        <v>10</v>
+      </c>
+      <c r="E28" s="13">
+        <v>3</v>
+      </c>
+      <c r="F28" s="13">
+        <v>13</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+      <c r="H28" t="str">
+        <f t="shared" si="1"/>
+        <v>true</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="13">
+        <v>20</v>
+      </c>
+      <c r="B29" s="13">
+        <v>3</v>
+      </c>
+      <c r="C29" s="13">
+        <v>23</v>
+      </c>
+      <c r="D29" s="13">
+        <v>12</v>
+      </c>
+      <c r="E29" s="13">
+        <v>5</v>
+      </c>
+      <c r="F29" s="13">
+        <v>17</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+      <c r="H29" t="str">
+        <f t="shared" si="1"/>
+        <v>true</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="13">
+        <v>20</v>
+      </c>
+      <c r="B30" s="13">
+        <v>3</v>
+      </c>
+      <c r="C30" s="13">
+        <v>23</v>
+      </c>
+      <c r="D30" s="13">
+        <v>16</v>
+      </c>
+      <c r="E30" s="13">
+        <v>2</v>
+      </c>
+      <c r="F30" s="13">
+        <v>18</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+      <c r="H30" t="str">
+        <f t="shared" si="1"/>
+        <v>true</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="13">
+        <v>20</v>
+      </c>
+      <c r="B31" s="13">
+        <v>3</v>
+      </c>
+      <c r="C31" s="13">
+        <v>23</v>
+      </c>
+      <c r="D31" s="13">
+        <v>20</v>
+      </c>
+      <c r="E31" s="13">
+        <v>3</v>
+      </c>
+      <c r="F31" s="13">
+        <v>23</v>
+      </c>
+      <c r="G31" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>Conflito</v>
+      </c>
+      <c r="H31" s="16" t="str">
+        <f t="shared" si="1"/>
+        <v>false</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="13">
+        <v>20</v>
+      </c>
+      <c r="B32" s="13">
+        <v>3</v>
+      </c>
+      <c r="C32" s="13">
+        <v>23</v>
+      </c>
+      <c r="D32" s="13">
+        <v>21</v>
+      </c>
+      <c r="E32" s="13">
+        <v>0</v>
+      </c>
+      <c r="F32" s="13">
+        <v>21</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+      <c r="H32" t="str">
+        <f t="shared" si="1"/>
+        <v>true</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="14">
+        <v>21</v>
+      </c>
+      <c r="B33" s="14">
+        <v>0</v>
+      </c>
+      <c r="C33" s="14">
+        <v>21</v>
+      </c>
+      <c r="D33" s="14">
+        <v>7</v>
+      </c>
+      <c r="E33" s="14">
+        <v>1</v>
+      </c>
+      <c r="F33" s="14">
+        <v>8</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+      <c r="H33" t="str">
+        <f t="shared" si="1"/>
+        <v>true</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="14">
+        <v>21</v>
+      </c>
+      <c r="B34" s="14">
+        <v>0</v>
+      </c>
+      <c r="C34" s="14">
+        <v>21</v>
+      </c>
+      <c r="D34" s="14">
+        <v>10</v>
+      </c>
+      <c r="E34" s="14">
+        <v>3</v>
+      </c>
+      <c r="F34" s="14">
+        <v>13</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+      <c r="H34" t="str">
+        <f t="shared" si="1"/>
+        <v>true</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="14">
+        <v>21</v>
+      </c>
+      <c r="B35" s="14">
+        <v>0</v>
+      </c>
+      <c r="C35" s="14">
+        <v>21</v>
+      </c>
+      <c r="D35" s="14">
+        <v>12</v>
+      </c>
+      <c r="E35" s="14">
+        <v>5</v>
+      </c>
+      <c r="F35" s="14">
+        <v>17</v>
+      </c>
+      <c r="G35" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+      <c r="H35" t="str">
+        <f t="shared" si="1"/>
+        <v>true</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" s="14">
+        <v>21</v>
+      </c>
+      <c r="B36" s="14">
+        <v>0</v>
+      </c>
+      <c r="C36" s="14">
+        <v>21</v>
+      </c>
+      <c r="D36" s="14">
+        <v>16</v>
+      </c>
+      <c r="E36" s="14">
+        <v>2</v>
+      </c>
+      <c r="F36" s="14">
+        <v>18</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+      <c r="H36" t="str">
+        <f t="shared" si="1"/>
+        <v>true</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" s="14">
+        <v>21</v>
+      </c>
+      <c r="B37" s="14">
+        <v>0</v>
+      </c>
+      <c r="C37" s="14">
+        <v>21</v>
+      </c>
+      <c r="D37" s="14">
+        <v>20</v>
+      </c>
+      <c r="E37" s="14">
+        <v>3</v>
+      </c>
+      <c r="F37" s="14">
+        <v>23</v>
+      </c>
+      <c r="G37" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+      <c r="H37" t="str">
+        <f t="shared" si="1"/>
+        <v>true</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" s="14">
+        <v>21</v>
+      </c>
+      <c r="B38" s="14">
+        <v>0</v>
+      </c>
+      <c r="C38" s="14">
+        <v>21</v>
+      </c>
+      <c r="D38" s="14">
+        <v>21</v>
+      </c>
+      <c r="E38" s="14">
+        <v>0</v>
+      </c>
+      <c r="F38" s="14">
+        <v>21</v>
+      </c>
+      <c r="G38" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>OK</v>
+      </c>
+      <c r="H38" s="16" t="str">
+        <f t="shared" si="1"/>
+        <v>true</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B260754-0212-467D-A128-42BD99D7EFB6}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
@@ -548,16 +1679,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6" t="s">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
       <c r="G1" s="1" t="s">
         <v>29</v>
       </c>
@@ -798,7 +1929,7 @@
         <v>2</v>
       </c>
       <c r="F9" s="5">
-        <f t="shared" ref="F9:F14" si="6">D9+E9</f>
+        <f t="shared" ref="F9:F13" si="6">D9+E9</f>
         <v>10</v>
       </c>
       <c r="G9" t="b">
@@ -909,23 +2040,23 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="8">
+      <c r="A13" s="7">
         <v>11</v>
       </c>
-      <c r="B13" s="8">
-        <v>0</v>
-      </c>
-      <c r="C13" s="8">
+      <c r="B13" s="7">
+        <v>0</v>
+      </c>
+      <c r="C13" s="7">
         <f t="shared" si="5"/>
         <v>11</v>
       </c>
-      <c r="D13" s="7">
-        <v>12</v>
-      </c>
-      <c r="E13" s="7">
-        <v>2</v>
-      </c>
-      <c r="F13" s="7">
+      <c r="D13" s="6">
+        <v>12</v>
+      </c>
+      <c r="E13" s="6">
+        <v>2</v>
+      </c>
+      <c r="F13" s="6">
         <f t="shared" si="6"/>
         <v>14</v>
       </c>
@@ -941,23 +2072,23 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="8">
-        <v>12</v>
-      </c>
-      <c r="B14" s="8">
-        <v>0</v>
-      </c>
-      <c r="C14" s="8">
+      <c r="A14" s="7">
+        <v>12</v>
+      </c>
+      <c r="B14" s="7">
+        <v>0</v>
+      </c>
+      <c r="C14" s="7">
         <f t="shared" si="5"/>
         <v>12</v>
       </c>
-      <c r="D14" s="7">
-        <v>12</v>
-      </c>
-      <c r="E14" s="7">
-        <v>2</v>
-      </c>
-      <c r="F14" s="7">
+      <c r="D14" s="6">
+        <v>12</v>
+      </c>
+      <c r="E14" s="6">
+        <v>2</v>
+      </c>
+      <c r="F14" s="6">
         <f t="shared" ref="F14:F22" si="7">D14+E14</f>
         <v>14</v>
       </c>
@@ -973,23 +2104,23 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="8">
+      <c r="A15" s="7">
         <v>13</v>
       </c>
-      <c r="B15" s="8">
-        <v>0</v>
-      </c>
-      <c r="C15" s="8">
+      <c r="B15" s="7">
+        <v>0</v>
+      </c>
+      <c r="C15" s="7">
         <f t="shared" si="5"/>
         <v>13</v>
       </c>
-      <c r="D15" s="7">
-        <v>12</v>
-      </c>
-      <c r="E15" s="7">
-        <v>2</v>
-      </c>
-      <c r="F15" s="7">
+      <c r="D15" s="6">
+        <v>12</v>
+      </c>
+      <c r="E15" s="6">
+        <v>2</v>
+      </c>
+      <c r="F15" s="6">
         <f t="shared" si="7"/>
         <v>14</v>
       </c>
@@ -1005,23 +2136,23 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="8">
+      <c r="A16" s="7">
         <v>14</v>
       </c>
-      <c r="B16" s="8">
-        <v>0</v>
-      </c>
-      <c r="C16" s="8">
+      <c r="B16" s="7">
+        <v>0</v>
+      </c>
+      <c r="C16" s="7">
         <f t="shared" si="5"/>
         <v>14</v>
       </c>
-      <c r="D16" s="7">
-        <v>12</v>
-      </c>
-      <c r="E16" s="7">
-        <v>2</v>
-      </c>
-      <c r="F16" s="7">
+      <c r="D16" s="6">
+        <v>12</v>
+      </c>
+      <c r="E16" s="6">
+        <v>2</v>
+      </c>
+      <c r="F16" s="6">
         <f t="shared" si="7"/>
         <v>14</v>
       </c>
@@ -1037,23 +2168,23 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="8">
+      <c r="A17" s="7">
         <v>15</v>
       </c>
-      <c r="B17" s="8">
-        <v>0</v>
-      </c>
-      <c r="C17" s="8">
+      <c r="B17" s="7">
+        <v>0</v>
+      </c>
+      <c r="C17" s="7">
         <f t="shared" si="5"/>
         <v>15</v>
       </c>
-      <c r="D17" s="7">
-        <v>12</v>
-      </c>
-      <c r="E17" s="7">
-        <v>2</v>
-      </c>
-      <c r="F17" s="7">
+      <c r="D17" s="6">
+        <v>12</v>
+      </c>
+      <c r="E17" s="6">
+        <v>2</v>
+      </c>
+      <c r="F17" s="6">
         <f t="shared" si="7"/>
         <v>14</v>
       </c>
@@ -1069,23 +2200,23 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="7">
-        <v>12</v>
-      </c>
-      <c r="B18" s="7">
-        <v>2</v>
-      </c>
-      <c r="C18" s="7">
+      <c r="A18" s="6">
+        <v>12</v>
+      </c>
+      <c r="B18" s="6">
+        <v>2</v>
+      </c>
+      <c r="C18" s="6">
         <f t="shared" si="5"/>
         <v>14</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D18" s="7">
         <v>11</v>
       </c>
-      <c r="E18" s="8">
-        <v>0</v>
-      </c>
-      <c r="F18" s="8">
+      <c r="E18" s="7">
+        <v>0</v>
+      </c>
+      <c r="F18" s="7">
         <f t="shared" si="7"/>
         <v>11</v>
       </c>
@@ -1101,23 +2232,23 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="7">
-        <v>12</v>
-      </c>
-      <c r="B19" s="7">
-        <v>2</v>
-      </c>
-      <c r="C19" s="7">
+      <c r="A19" s="6">
+        <v>12</v>
+      </c>
+      <c r="B19" s="6">
+        <v>2</v>
+      </c>
+      <c r="C19" s="6">
         <f t="shared" si="5"/>
         <v>14</v>
       </c>
-      <c r="D19" s="8">
-        <v>12</v>
-      </c>
-      <c r="E19" s="8">
-        <v>0</v>
-      </c>
-      <c r="F19" s="8">
+      <c r="D19" s="7">
+        <v>12</v>
+      </c>
+      <c r="E19" s="7">
+        <v>0</v>
+      </c>
+      <c r="F19" s="7">
         <f t="shared" si="7"/>
         <v>12</v>
       </c>
@@ -1133,23 +2264,23 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="7">
-        <v>12</v>
-      </c>
-      <c r="B20" s="7">
-        <v>2</v>
-      </c>
-      <c r="C20" s="7">
+      <c r="A20" s="6">
+        <v>12</v>
+      </c>
+      <c r="B20" s="6">
+        <v>2</v>
+      </c>
+      <c r="C20" s="6">
         <f t="shared" si="5"/>
         <v>14</v>
       </c>
-      <c r="D20" s="8">
+      <c r="D20" s="7">
         <v>13</v>
       </c>
-      <c r="E20" s="8">
-        <v>0</v>
-      </c>
-      <c r="F20" s="8">
+      <c r="E20" s="7">
+        <v>0</v>
+      </c>
+      <c r="F20" s="7">
         <f t="shared" si="7"/>
         <v>13</v>
       </c>
@@ -1165,23 +2296,23 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="7">
-        <v>12</v>
-      </c>
-      <c r="B21" s="7">
-        <v>2</v>
-      </c>
-      <c r="C21" s="7">
+      <c r="A21" s="6">
+        <v>12</v>
+      </c>
+      <c r="B21" s="6">
+        <v>2</v>
+      </c>
+      <c r="C21" s="6">
         <f t="shared" si="5"/>
         <v>14</v>
       </c>
-      <c r="D21" s="8">
+      <c r="D21" s="7">
         <v>14</v>
       </c>
-      <c r="E21" s="8">
-        <v>0</v>
-      </c>
-      <c r="F21" s="8">
+      <c r="E21" s="7">
+        <v>0</v>
+      </c>
+      <c r="F21" s="7">
         <f t="shared" si="7"/>
         <v>14</v>
       </c>
@@ -1197,23 +2328,23 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="7">
-        <v>12</v>
-      </c>
-      <c r="B22" s="7">
-        <v>2</v>
-      </c>
-      <c r="C22" s="7">
+      <c r="A22" s="6">
+        <v>12</v>
+      </c>
+      <c r="B22" s="6">
+        <v>2</v>
+      </c>
+      <c r="C22" s="6">
         <f t="shared" si="5"/>
         <v>14</v>
       </c>
-      <c r="D22" s="8">
+      <c r="D22" s="7">
         <v>15</v>
       </c>
-      <c r="E22" s="8">
-        <v>0</v>
-      </c>
-      <c r="F22" s="8">
+      <c r="E22" s="7">
+        <v>0</v>
+      </c>
+      <c r="F22" s="7">
         <f t="shared" si="7"/>
         <v>15</v>
       </c>

</xml_diff>